<commit_message>
Se arreglaron errores del analizador lexico, y unos errores del pintador, incorporacion del analizador sintactico, sin embargo checar para errores
</commit_message>
<xml_diff>
--- a/Tabla Transiciones.xlsx
+++ b/Tabla Transiciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camran1234\source\repos\Proyecto2_Lenguajes_Analizador_Sintactico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641E3943-3F8E-48A6-81B3-BE8B46075B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A227237-2C79-4A66-AC83-8607A9310B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7B0EC626-8F7A-4356-909D-4F40060FBAEF}"/>
+    <workbookView xWindow="14316" yWindow="4656" windowWidth="17280" windowHeight="8964" xr2:uid="{7B0EC626-8F7A-4356-909D-4F40060FBAEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="137">
   <si>
     <t>E</t>
   </si>
@@ -204,9 +204,6 @@
     <t>cadena</t>
   </si>
   <si>
-    <t>char</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
@@ -381,9 +378,6 @@
     <t>DESDE VX</t>
   </si>
   <si>
-    <t>=WB</t>
-  </si>
-  <si>
     <t>=W B</t>
   </si>
   <si>
@@ -414,9 +408,6 @@
     <t>Leer Pa V</t>
   </si>
   <si>
-    <t>W C</t>
-  </si>
-  <si>
     <t>G_MQ</t>
   </si>
   <si>
@@ -436,6 +427,15 @@
   </si>
   <si>
     <t>_W C</t>
+  </si>
+  <si>
+    <t>char'</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Hasta V _B</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -508,6 +508,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF434BF-CB45-4D43-9B6B-74558F129D5D}">
-  <dimension ref="C5:AR49"/>
+  <dimension ref="B5:AR48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="S4" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="V48" sqref="V48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,11 +835,12 @@
     <col min="12" max="12" width="14.109375" customWidth="1"/>
     <col min="15" max="15" width="14.88671875" customWidth="1"/>
     <col min="16" max="16" width="20.44140625" customWidth="1"/>
+    <col min="17" max="17" width="21.44140625" customWidth="1"/>
     <col min="23" max="23" width="14.109375" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" customWidth="1"/>
+    <col min="35" max="35" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:44" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
         <v>42</v>
@@ -859,10 +861,10 @@
         <v>47</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>48</v>
@@ -874,10 +876,10 @@
         <v>50</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>51</v>
@@ -898,73 +900,76 @@
         <v>56</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X5" s="2" t="s">
         <v>57</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="Z5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AB5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AB5" s="2" t="s">
+      <c r="AC5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AD5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="AF5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AF5" s="3" t="s">
+      <c r="AG5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AG5" s="2" t="s">
+      <c r="AH5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AH5" s="2" t="s">
+      <c r="AI5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AI5" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="AJ5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AK5" s="2" t="s">
+      <c r="AL5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AL5" s="2" t="s">
+      <c r="AM5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AM5" s="2" t="s">
+      <c r="AN5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AN5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AO5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AP5" s="2" t="s">
+      <c r="AQ5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AQ5" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="AR5" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="3:44" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>1</v>
+      </c>
       <c r="C6" s="4" t="s">
         <v>0</v>
       </c>
@@ -988,7 +993,7 @@
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
@@ -1010,11 +1015,12 @@
       <c r="AO6" s="5"/>
       <c r="AP6" s="5"/>
       <c r="AQ6" s="5"/>
-      <c r="AR6" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="3:44" x14ac:dyDescent="0.3">
+      <c r="AR6" s="5"/>
+    </row>
+    <row r="7" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>2</v>
+      </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
@@ -1038,7 +1044,7 @@
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
@@ -1062,7 +1068,10 @@
       <c r="AQ7" s="5"/>
       <c r="AR7" s="5"/>
     </row>
-    <row r="8" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>3</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1110,7 +1119,10 @@
       <c r="AQ8" s="5"/>
       <c r="AR8" s="5"/>
     </row>
-    <row r="9" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>4</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1158,46 +1170,49 @@
       <c r="AQ9" s="5"/>
       <c r="AR9" s="5"/>
     </row>
-    <row r="10" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>5</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="R10" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="S10" s="5"/>
       <c r="T10" s="5" t="s">
@@ -1228,7 +1243,10 @@
       <c r="AQ10" s="5"/>
       <c r="AR10" s="5"/>
     </row>
-    <row r="11" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>6</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
@@ -1276,7 +1294,10 @@
       <c r="AQ11" s="5"/>
       <c r="AR11" s="5"/>
     </row>
-    <row r="12" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>7</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>6</v>
       </c>
@@ -1324,24 +1345,27 @@
       <c r="AQ12" s="5"/>
       <c r="AR12" s="5"/>
     </row>
-    <row r="13" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>8</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1380,24 +1404,27 @@
       <c r="AQ13" s="5"/>
       <c r="AR13" s="5"/>
     </row>
-    <row r="14" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>9</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1436,7 +1463,10 @@
       <c r="AQ14" s="5"/>
       <c r="AR14" s="5"/>
     </row>
-    <row r="15" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>10</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -1461,25 +1491,25 @@
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AB15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AD15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AE15" s="5"/>
       <c r="AF15" s="5"/>
@@ -1496,7 +1526,10 @@
       <c r="AQ15" s="5"/>
       <c r="AR15" s="5"/>
     </row>
-    <row r="16" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>11</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
@@ -1527,7 +1560,7 @@
       <c r="AB16" s="5"/>
       <c r="AC16" s="5"/>
       <c r="AD16" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AE16" s="5"/>
       <c r="AF16" s="5"/>
@@ -1544,7 +1577,10 @@
       <c r="AQ16" s="5"/>
       <c r="AR16" s="5"/>
     </row>
-    <row r="17" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>12</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>11</v>
       </c>
@@ -1576,11 +1612,11 @@
       <c r="AC17" s="5"/>
       <c r="AD17" s="5"/>
       <c r="AE17" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AF17" s="5"/>
       <c r="AG17" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH17" s="5"/>
       <c r="AI17" s="5"/>
@@ -1594,7 +1630,10 @@
       <c r="AQ17" s="5"/>
       <c r="AR17" s="5"/>
     </row>
-    <row r="18" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>13</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
@@ -1629,7 +1668,7 @@
       <c r="AF18" s="5"/>
       <c r="AG18" s="5"/>
       <c r="AH18" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI18" s="5"/>
       <c r="AJ18" s="5"/>
@@ -1642,7 +1681,10 @@
       <c r="AQ18" s="5"/>
       <c r="AR18" s="5"/>
     </row>
-    <row r="19" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>14</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>13</v>
       </c>
@@ -1676,10 +1718,10 @@
       <c r="AE19" s="5"/>
       <c r="AF19" s="5"/>
       <c r="AG19" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH19" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI19" s="5"/>
       <c r="AJ19" s="5"/>
@@ -1692,7 +1734,10 @@
       <c r="AQ19" s="5"/>
       <c r="AR19" s="5"/>
     </row>
-    <row r="20" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>15</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>14</v>
       </c>
@@ -1717,25 +1762,25 @@
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE20" s="5"/>
       <c r="AF20" s="5"/>
@@ -1752,7 +1797,10 @@
       <c r="AQ20" s="5"/>
       <c r="AR20" s="5"/>
     </row>
-    <row r="21" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>16</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>15</v>
       </c>
@@ -1787,10 +1835,10 @@
       <c r="AF21" s="5"/>
       <c r="AG21" s="5"/>
       <c r="AH21" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI21" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AJ21" s="5"/>
       <c r="AK21" s="5"/>
@@ -1802,7 +1850,10 @@
       <c r="AQ21" s="5"/>
       <c r="AR21" s="5"/>
     </row>
-    <row r="22" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>17</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>16</v>
       </c>
@@ -1812,7 +1863,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -1850,7 +1901,10 @@
       <c r="AQ22" s="5"/>
       <c r="AR22" s="5"/>
     </row>
-    <row r="23" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>18</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>17</v>
       </c>
@@ -1870,7 +1924,7 @@
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
@@ -1898,7 +1952,10 @@
       <c r="AQ23" s="5"/>
       <c r="AR23" s="5"/>
     </row>
-    <row r="24" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>19</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1908,7 +1965,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -1946,54 +2003,57 @@
       <c r="AQ24" s="5"/>
       <c r="AR24" s="5"/>
     </row>
-    <row r="25" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>20</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J25" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K25" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="L25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S25" s="5"/>
       <c r="T25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
@@ -2020,7 +2080,10 @@
       <c r="AQ25" s="5"/>
       <c r="AR25" s="5"/>
     </row>
-    <row r="26" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>21</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>20</v>
       </c>
@@ -2033,7 +2096,7 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
@@ -2068,7 +2131,10 @@
       <c r="AQ26" s="5"/>
       <c r="AR26" s="5"/>
     </row>
-    <row r="27" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>22</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>21</v>
       </c>
@@ -2081,7 +2147,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
@@ -2116,7 +2182,10 @@
       <c r="AQ27" s="5"/>
       <c r="AR27" s="5"/>
     </row>
-    <row r="28" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>23</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>22</v>
       </c>
@@ -2136,7 +2205,7 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
@@ -2164,7 +2233,10 @@
       <c r="AQ28" s="5"/>
       <c r="AR28" s="5"/>
     </row>
-    <row r="29" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>24</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>23</v>
       </c>
@@ -2178,7 +2250,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
@@ -2212,7 +2284,10 @@
       <c r="AQ29" s="5"/>
       <c r="AR29" s="5"/>
     </row>
-    <row r="30" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>25</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>24</v>
       </c>
@@ -2226,7 +2301,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
@@ -2260,50 +2335,53 @@
       <c r="AQ30" s="5"/>
       <c r="AR30" s="5"/>
     </row>
-    <row r="31" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>26</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="R31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="S31" s="5"/>
       <c r="T31" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
@@ -2330,7 +2408,10 @@
       <c r="AQ31" s="5"/>
       <c r="AR31" s="5"/>
     </row>
-    <row r="32" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>27</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>26</v>
       </c>
@@ -2355,25 +2436,25 @@
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
       <c r="X32" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Y32" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z32" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AA32" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AB32" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AC32" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AD32" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AE32" s="5"/>
       <c r="AF32" s="5"/>
@@ -2385,16 +2466,19 @@
       <c r="AL32" s="5"/>
       <c r="AM32" s="5"/>
       <c r="AN32" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AO32" s="5"/>
       <c r="AP32" s="5"/>
       <c r="AQ32" s="5"/>
       <c r="AR32" s="5"/>
     </row>
-    <row r="33" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>28</v>
+      </c>
       <c r="C33" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -2433,14 +2517,17 @@
       <c r="AL33" s="5"/>
       <c r="AM33" s="5"/>
       <c r="AN33" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AO33" s="5"/>
       <c r="AP33" s="5"/>
       <c r="AQ33" s="5"/>
       <c r="AR33" s="5"/>
     </row>
-    <row r="34" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>29</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>27</v>
       </c>
@@ -2471,16 +2558,16 @@
         <v>58</v>
       </c>
       <c r="Z34" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AA34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB34" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AB34" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="AC34" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD34" s="5" t="s">
         <v>10</v>
@@ -2500,7 +2587,10 @@
       <c r="AQ34" s="5"/>
       <c r="AR34" s="5"/>
     </row>
-    <row r="35" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>30</v>
+      </c>
       <c r="C35" s="4" t="s">
         <v>28</v>
       </c>
@@ -2523,7 +2613,7 @@
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
       <c r="V35" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W35" s="5"/>
       <c r="X35" s="5"/>
@@ -2535,34 +2625,37 @@
       <c r="AD35" s="5"/>
       <c r="AE35" s="5"/>
       <c r="AF35" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AG35" s="5"/>
       <c r="AH35" s="5"/>
       <c r="AI35" s="5"/>
       <c r="AJ35" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK35" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AK35" s="5" t="s">
+      <c r="AL35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AL35" s="5" t="s">
+      <c r="AM35" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="AM35" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="AN35" s="5"/>
       <c r="AO35" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AP35" s="5"/>
       <c r="AQ35" s="5"/>
       <c r="AR35" s="5"/>
     </row>
-    <row r="36" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>31</v>
+      </c>
       <c r="C36" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -2582,29 +2675,17 @@
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
       <c r="U36" s="5"/>
-      <c r="V36" s="5"/>
+      <c r="V36" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="W36" s="5"/>
-      <c r="X36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="AA36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="AB36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="AD36" s="5" t="s">
-        <v>129</v>
-      </c>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="5"/>
+      <c r="AC36" s="5"/>
+      <c r="AD36" s="5"/>
       <c r="AE36" s="5"/>
       <c r="AF36" s="5"/>
       <c r="AG36" s="5"/>
@@ -2616,13 +2697,20 @@
       <c r="AM36" s="5"/>
       <c r="AN36" s="5"/>
       <c r="AO36" s="5"/>
-      <c r="AP36" s="5"/>
-      <c r="AQ36" s="5"/>
+      <c r="AP36" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ36" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="AR36" s="5"/>
     </row>
-    <row r="37" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>32</v>
+      </c>
       <c r="C37" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -2634,7 +2722,9 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
+      <c r="N37" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
@@ -2642,9 +2732,7 @@
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
       <c r="U37" s="5"/>
-      <c r="V37" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="V37" s="5"/>
       <c r="W37" s="5"/>
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
@@ -2664,17 +2752,16 @@
       <c r="AM37" s="5"/>
       <c r="AN37" s="5"/>
       <c r="AO37" s="5"/>
-      <c r="AP37" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AQ37" s="5" t="s">
-        <v>116</v>
-      </c>
+      <c r="AP37" s="5"/>
+      <c r="AQ37" s="5"/>
       <c r="AR37" s="5"/>
     </row>
-    <row r="38" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>33</v>
+      </c>
       <c r="C38" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -2686,9 +2773,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
-      <c r="N38" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
@@ -2705,7 +2790,9 @@
       <c r="AB38" s="5"/>
       <c r="AC38" s="5"/>
       <c r="AD38" s="5"/>
-      <c r="AE38" s="5"/>
+      <c r="AE38" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="AF38" s="5"/>
       <c r="AG38" s="5"/>
       <c r="AH38" s="5"/>
@@ -2720,9 +2807,12 @@
       <c r="AQ38" s="5"/>
       <c r="AR38" s="5"/>
     </row>
-    <row r="39" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>34</v>
+      </c>
       <c r="C39" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -2735,7 +2825,9 @@
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
+      <c r="O39" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
@@ -2751,9 +2843,7 @@
       <c r="AB39" s="5"/>
       <c r="AC39" s="5"/>
       <c r="AD39" s="5"/>
-      <c r="AE39" s="6" t="s">
-        <v>119</v>
-      </c>
+      <c r="AE39" s="6"/>
       <c r="AF39" s="5"/>
       <c r="AG39" s="5"/>
       <c r="AH39" s="5"/>
@@ -2768,9 +2858,12 @@
       <c r="AQ39" s="5"/>
       <c r="AR39" s="5"/>
     </row>
-    <row r="40" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>35</v>
+      </c>
       <c r="C40" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -2790,7 +2883,7 @@
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
       <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
+      <c r="V40" s="7"/>
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
@@ -2799,26 +2892,39 @@
       <c r="AB40" s="5"/>
       <c r="AC40" s="5"/>
       <c r="AD40" s="5"/>
-      <c r="AE40" s="6" t="s">
+      <c r="AE40" s="5"/>
+      <c r="AF40" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="AF40" s="5"/>
       <c r="AG40" s="5"/>
       <c r="AH40" s="5"/>
       <c r="AI40" s="5"/>
-      <c r="AJ40" s="5"/>
-      <c r="AK40" s="5"/>
-      <c r="AL40" s="5"/>
-      <c r="AM40" s="5"/>
+      <c r="AJ40" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK40" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL40" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM40" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="AN40" s="5"/>
-      <c r="AO40" s="5"/>
+      <c r="AO40" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="AP40" s="5"/>
       <c r="AQ40" s="5"/>
       <c r="AR40" s="5"/>
     </row>
-    <row r="41" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>36</v>
+      </c>
       <c r="C41" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -2832,7 +2938,9 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
+      <c r="P41" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
@@ -2848,35 +2956,26 @@
       <c r="AC41" s="5"/>
       <c r="AD41" s="5"/>
       <c r="AE41" s="5"/>
-      <c r="AF41" s="5" t="s">
-        <v>120</v>
-      </c>
+      <c r="AF41" s="5"/>
       <c r="AG41" s="5"/>
       <c r="AH41" s="5"/>
       <c r="AI41" s="5"/>
-      <c r="AJ41" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK41" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL41" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AM41" s="5" t="s">
-        <v>120</v>
-      </c>
+      <c r="AJ41" s="5"/>
+      <c r="AK41" s="5"/>
+      <c r="AL41" s="5"/>
+      <c r="AM41" s="5"/>
       <c r="AN41" s="5"/>
-      <c r="AO41" s="5" t="s">
-        <v>120</v>
-      </c>
+      <c r="AO41" s="5"/>
       <c r="AP41" s="5"/>
       <c r="AQ41" s="5"/>
       <c r="AR41" s="5"/>
     </row>
-    <row r="42" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>37</v>
+      </c>
       <c r="C42" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -2890,12 +2989,12 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
-      <c r="P42" s="5" t="s">
-        <v>121</v>
-      </c>
+      <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
+      <c r="S42" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="T42" s="5"/>
       <c r="U42" s="5"/>
       <c r="V42" s="5"/>
@@ -2922,9 +3021,12 @@
       <c r="AQ42" s="5"/>
       <c r="AR42" s="5"/>
     </row>
-    <row r="43" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>38</v>
+      </c>
       <c r="C43" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -2939,11 +3041,11 @@
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
+      <c r="Q43" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="R43" s="5"/>
-      <c r="S43" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="S43" s="5"/>
       <c r="T43" s="5"/>
       <c r="U43" s="5"/>
       <c r="V43" s="5"/>
@@ -2970,9 +3072,12 @@
       <c r="AQ43" s="5"/>
       <c r="AR43" s="5"/>
     </row>
-    <row r="44" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>39</v>
+      </c>
       <c r="C44" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -2987,14 +3092,14 @@
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
-      <c r="Q44" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
       <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
+      <c r="V44" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="W44" s="5"/>
       <c r="X44" s="5"/>
       <c r="Y44" s="5"/>
@@ -3007,7 +3112,9 @@
       <c r="AF44" s="5"/>
       <c r="AG44" s="5"/>
       <c r="AH44" s="5"/>
-      <c r="AI44" s="5"/>
+      <c r="AI44" s="6" t="s">
+        <v>122</v>
+      </c>
       <c r="AJ44" s="5"/>
       <c r="AK44" s="5"/>
       <c r="AL44" s="5"/>
@@ -3018,9 +3125,12 @@
       <c r="AQ44" s="5"/>
       <c r="AR44" s="5"/>
     </row>
-    <row r="45" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>40</v>
+      </c>
       <c r="C45" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -3035,14 +3145,14 @@
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
+      <c r="Q45" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="R45" s="5"/>
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
       <c r="U45" s="5"/>
-      <c r="V45" s="5" t="s">
-        <v>126</v>
-      </c>
+      <c r="V45" s="5"/>
       <c r="W45" s="5"/>
       <c r="X45" s="5"/>
       <c r="Y45" s="5"/>
@@ -3055,9 +3165,7 @@
       <c r="AF45" s="5"/>
       <c r="AG45" s="5"/>
       <c r="AH45" s="5"/>
-      <c r="AI45" s="6" t="s">
-        <v>124</v>
-      </c>
+      <c r="AI45" s="5"/>
       <c r="AJ45" s="5"/>
       <c r="AK45" s="5"/>
       <c r="AL45" s="5"/>
@@ -3068,9 +3176,12 @@
       <c r="AQ45" s="5"/>
       <c r="AR45" s="5"/>
     </row>
-    <row r="46" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>41</v>
+      </c>
       <c r="C46" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -3086,7 +3197,9 @@
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
+      <c r="R46" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
@@ -3103,9 +3216,7 @@
       <c r="AF46" s="5"/>
       <c r="AG46" s="5"/>
       <c r="AH46" s="5"/>
-      <c r="AI46" s="5" t="s">
-        <v>125</v>
-      </c>
+      <c r="AI46" s="5"/>
       <c r="AJ46" s="5"/>
       <c r="AK46" s="5"/>
       <c r="AL46" s="5"/>
@@ -3116,9 +3227,12 @@
       <c r="AQ46" s="5"/>
       <c r="AR46" s="5"/>
     </row>
-    <row r="47" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>42</v>
+      </c>
       <c r="C47" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -3135,7 +3249,7 @@
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
@@ -3164,9 +3278,12 @@
       <c r="AQ47" s="5"/>
       <c r="AR47" s="5"/>
     </row>
-    <row r="48" spans="3:44" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>43</v>
+      </c>
       <c r="C48" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -3182,13 +3299,13 @@
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
-      <c r="R48" s="5" t="s">
-        <v>128</v>
-      </c>
+      <c r="R48" s="5"/>
       <c r="S48" s="5"/>
       <c r="T48" s="5"/>
       <c r="U48" s="5"/>
-      <c r="V48" s="5"/>
+      <c r="V48" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="W48" s="5"/>
       <c r="X48" s="5"/>
       <c r="Y48" s="5"/>
@@ -3212,54 +3329,6 @@
       <c r="AQ48" s="5"/>
       <c r="AR48" s="5"/>
     </row>
-    <row r="49" spans="3:44" x14ac:dyDescent="0.3">
-      <c r="C49" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="5"/>
-      <c r="U49" s="5"/>
-      <c r="V49" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="W49" s="5"/>
-      <c r="X49" s="5"/>
-      <c r="Y49" s="5"/>
-      <c r="Z49" s="5"/>
-      <c r="AA49" s="5"/>
-      <c r="AB49" s="5"/>
-      <c r="AC49" s="5"/>
-      <c r="AD49" s="5"/>
-      <c r="AE49" s="5"/>
-      <c r="AF49" s="5"/>
-      <c r="AG49" s="5"/>
-      <c r="AH49" s="5"/>
-      <c r="AI49" s="5"/>
-      <c r="AJ49" s="5"/>
-      <c r="AK49" s="5"/>
-      <c r="AL49" s="5"/>
-      <c r="AM49" s="5"/>
-      <c r="AN49" s="5"/>
-      <c r="AO49" s="5"/>
-      <c r="AP49" s="5"/>
-      <c r="AQ49" s="5"/>
-      <c r="AR49" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>